<commit_message>
Dump of everything from media folder - don't have time to sort it out now, have to return laptop
</commit_message>
<xml_diff>
--- a/media/spreadsheets/Timing.xlsx
+++ b/media/spreadsheets/Timing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Visualization" sheetId="1" r:id="rId1"/>
@@ -1234,11 +1234,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="91691264"/>
-        <c:axId val="150533632"/>
+        <c:axId val="41171968"/>
+        <c:axId val="41182336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91691264"/>
+        <c:axId val="41171968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1273,7 +1273,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150533632"/>
+        <c:crossAx val="41182336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1281,7 +1281,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150533632"/>
+        <c:axId val="41182336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1319,7 +1319,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91691264"/>
+        <c:crossAx val="41171968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1659,11 +1659,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="173002752"/>
-        <c:axId val="187216640"/>
+        <c:axId val="41107840"/>
+        <c:axId val="41109760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="173002752"/>
+        <c:axId val="41107840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1698,7 +1698,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="187216640"/>
+        <c:crossAx val="41109760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1706,7 +1706,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="187216640"/>
+        <c:axId val="41109760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1744,7 +1744,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173002752"/>
+        <c:crossAx val="41107840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2084,11 +2084,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="208545280"/>
-        <c:axId val="208547200"/>
+        <c:axId val="41155200"/>
+        <c:axId val="43524864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="208545280"/>
+        <c:axId val="41155200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2123,7 +2123,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="208547200"/>
+        <c:crossAx val="43524864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2131,7 +2131,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208547200"/>
+        <c:axId val="43524864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2169,7 +2169,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="208545280"/>
+        <c:crossAx val="41155200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2383,11 +2383,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="92307456"/>
-        <c:axId val="92309376"/>
+        <c:axId val="43664512"/>
+        <c:axId val="43666432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="92307456"/>
+        <c:axId val="43664512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2422,7 +2422,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92309376"/>
+        <c:crossAx val="43666432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2430,7 +2430,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92309376"/>
+        <c:axId val="43666432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2468,7 +2468,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92307456"/>
+        <c:crossAx val="43664512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2651,11 +2651,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="92322816"/>
-        <c:axId val="92324992"/>
+        <c:axId val="43705088"/>
+        <c:axId val="43707008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="92322816"/>
+        <c:axId val="43705088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2690,7 +2690,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92324992"/>
+        <c:crossAx val="43707008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2698,7 +2698,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92324992"/>
+        <c:axId val="43707008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70"/>
@@ -2736,7 +2736,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92322816"/>
+        <c:crossAx val="43705088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4151,7 +4151,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:D17"/>
     </sheetView>
   </sheetViews>
@@ -11475,7 +11475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>

</xml_diff>